<commit_message>
Activacion de Botones en FacturaCLI
</commit_message>
<xml_diff>
--- a/doc/Pruebas finales tsno.xlsx
+++ b/doc/Pruebas finales tsno.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Tropical\doc\"/>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="106">
   <si>
     <t>Aceptacion de Facturas</t>
   </si>
@@ -326,17 +326,29 @@
     <t>OK</t>
   </si>
   <si>
-    <t>validar botones exportar - NC</t>
+    <t>Al eliminar una línea no borra la Orden y recarga sin rango de fechas</t>
   </si>
   <si>
     <t>Hay dudas con las porciones que se devuelven a Central.</t>
+  </si>
+  <si>
+    <t>Validar estimación de costos y cantidades</t>
+  </si>
+  <si>
+    <t>Validar estado de la NC cuando es rechazada.</t>
+  </si>
+  <si>
+    <t>Validar acciones y estados</t>
+  </si>
+  <si>
+    <t>Validar inventario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -354,6 +366,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -390,12 +409,17 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -438,13 +462,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -461,26 +486,33 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
+  <cellStyles count="5">
+    <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
-    <cellStyle name="Texto explicativo" xfId="3" builtinId="53"/>
+    <cellStyle name="Texto explicativo" xfId="4" builtinId="53"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -496,7 +528,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -760,13 +792,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" style="8" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5546875" style="10" customWidth="1"/>
     <col min="2" max="2" width="35.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.6640625" customWidth="1"/>
     <col min="4" max="4" width="65" style="2" customWidth="1"/>
@@ -774,25 +806,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="D1" s="7">
+      <c r="D1" s="9">
         <f>A4/49</f>
-        <v>0.97959183673469385</v>
+        <v>0.8571428571428571</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="10">
+      <c r="A4" s="12">
         <f>SUM(A5:A53)</f>
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="9">
+      <c r="A5" s="11">
         <f>IF(D5="OK",1,0)</f>
         <v>1</v>
       </c>
@@ -809,7 +841,7 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="9">
+      <c r="A6" s="11">
         <f t="shared" ref="A6:A53" si="0">IF(D6="OK",1,0)</f>
         <v>1</v>
       </c>
@@ -826,7 +858,7 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="9">
+      <c r="A7" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -843,7 +875,7 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="9">
+      <c r="A8" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -860,7 +892,7 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="9">
+      <c r="A9" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -877,7 +909,7 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="9">
+      <c r="A10" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -894,24 +926,24 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="A11" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>99</v>
+      <c r="D11" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="9">
+      <c r="A12" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -928,24 +960,23 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B13" s="4" t="s">
+      <c r="A13" s="11">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="3" t="s">
         <v>99</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="9">
+      <c r="A14" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -962,41 +993,39 @@
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B15" s="4" t="s">
+      <c r="A15" s="11">
+        <v>0</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>99</v>
+      <c r="D15" s="7" t="s">
+        <v>104</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B16" s="4" t="s">
+      <c r="A16" s="11">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="3" t="s">
         <v>99</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="9">
+      <c r="A17" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1013,7 +1042,7 @@
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="9">
+      <c r="A18" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1030,7 +1059,7 @@
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="9">
+      <c r="A19" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1047,7 +1076,7 @@
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="9">
+      <c r="A20" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1064,7 +1093,7 @@
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="9">
+      <c r="A21" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1081,14 +1110,14 @@
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B22" s="11" t="s">
+      <c r="A22" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B22" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="13" t="s">
         <v>35</v>
       </c>
       <c r="D22" s="3" t="s">
@@ -1098,7 +1127,7 @@
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="9">
+      <c r="A23" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1115,7 +1144,7 @@
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="9">
+      <c r="A24" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1132,24 +1161,24 @@
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B25" s="1" t="s">
+      <c r="A25" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>99</v>
+      <c r="D25" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="9">
+      <c r="A26" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1166,7 +1195,7 @@
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="9">
+      <c r="A27" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1183,24 +1212,23 @@
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B28" s="4" t="s">
+      <c r="A28" s="11">
+        <v>1</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="3" t="s">
         <v>99</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="9">
+      <c r="A29" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1217,7 +1245,7 @@
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="9">
+      <c r="A30" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1234,7 +1262,7 @@
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="9">
+      <c r="A31" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1251,7 +1279,7 @@
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="9">
+      <c r="A32" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1268,7 +1296,7 @@
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="9">
+      <c r="A33" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1285,7 +1313,7 @@
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="9">
+      <c r="A34" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1302,7 +1330,7 @@
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="9">
+      <c r="A35" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1319,7 +1347,7 @@
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="9">
+      <c r="A36" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1336,26 +1364,26 @@
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B37" s="4" t="s">
+      <c r="A37" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E37" s="4" t="s">
+      <c r="D37" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E37" s="6" t="s">
         <v>101</v>
       </c>
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="9">
+      <c r="A38" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1372,41 +1400,39 @@
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B39" s="4" t="s">
+      <c r="A39" s="11">
+        <v>1</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="3" t="s">
         <v>99</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="B40" s="4" t="s">
+      <c r="A40" s="11">
+        <v>1</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>100</v>
+      <c r="D40" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="9">
+      <c r="A41" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1423,7 +1449,7 @@
       <c r="F41" s="1"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="9">
+      <c r="A42" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1440,7 +1466,7 @@
       <c r="F42" s="1"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="9">
+      <c r="A43" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1457,7 +1483,7 @@
       <c r="F43" s="1"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="9">
+      <c r="A44" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1474,7 +1500,7 @@
       <c r="F44" s="1"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="9">
+      <c r="A45" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1491,24 +1517,24 @@
       <c r="F45" s="1"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B46" s="1" t="s">
+      <c r="A46" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B46" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>99</v>
+      <c r="D46" s="7" t="s">
+        <v>105</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="9">
+      <c r="A47" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1525,7 +1551,7 @@
       <c r="F47" s="1"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="9">
+      <c r="A48" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1542,24 +1568,22 @@
       <c r="F48" s="1"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B49" s="1" t="s">
+      <c r="A49" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B49" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>99</v>
-      </c>
+      <c r="D49" s="7"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="9">
+      <c r="A50" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1576,24 +1600,22 @@
       <c r="F50" s="1"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B51" s="1" t="s">
+      <c r="A51" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B51" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>99</v>
-      </c>
+      <c r="D51" s="7"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="9">
+      <c r="A52" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1610,18 +1632,18 @@
       <c r="F52" s="1"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B53" s="4" t="s">
+      <c r="A53" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B53" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D53" s="5" t="s">
-        <v>99</v>
+      <c r="D53" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>

</xml_diff>